<commit_message>
sync with nearly finished report and video folder created
</commit_message>
<xml_diff>
--- a/analyse_fonction_niveau_d'eau_07m_s.xlsx
+++ b/analyse_fonction_niveau_d'eau_07m_s.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="672" yWindow="96" windowWidth="12132" windowHeight="5856"/>
@@ -15,7 +15,7 @@
     <definedName name="analyse_fonction_niveau_d_eau_07m_s_1" localSheetId="0">Feuil1!$A$1:$F$75</definedName>
     <definedName name="analyse_fonction_niveau_d_eau_07m_s_2" localSheetId="0">Feuil1!$A$77:$F$147</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="12">
   <si>
     <t>root</t>
   </si>
@@ -80,18 +80,48 @@
   <si>
     <t>pelvis torso</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>φ=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <t>φ=1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -114,8 +144,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -144,6 +175,30 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>pelvis, axe</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> x</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -350,37 +405,85 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="233313408"/>
-        <c:axId val="233257216"/>
+        <c:axId val="132163072"/>
+        <c:axId val="132164608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="233313408"/>
+        <c:axId val="132163072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>niveau d'eau (en mètres)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1000">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="233257216"/>
+        <c:crossAx val="132164608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="233257216"/>
+        <c:axId val="132164608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>angle (en radians)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1000">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="233313408"/>
+        <c:crossAx val="132163072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -396,8 +499,8 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="1.3149999999999999" header="0.3" footer="0.3"/>
+    <c:pageSetup paperSize="9" orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -930,11 +1033,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="241387776"/>
-        <c:axId val="241386240"/>
+        <c:axId val="236435328"/>
+        <c:axId val="236436864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="241387776"/>
+        <c:axId val="236435328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -944,12 +1047,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="241386240"/>
+        <c:crossAx val="236436864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="241386240"/>
+        <c:axId val="236436864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -960,7 +1063,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="241387776"/>
+        <c:crossAx val="236435328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1270,11 +1373,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="246615424"/>
-        <c:axId val="242682112"/>
+        <c:axId val="236525824"/>
+        <c:axId val="236527616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="246615424"/>
+        <c:axId val="236525824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1284,12 +1387,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="242682112"/>
+        <c:crossAx val="236527616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="242682112"/>
+        <c:axId val="236527616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1300,7 +1403,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="246615424"/>
+        <c:crossAx val="236525824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1670,11 +1773,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="248142848"/>
-        <c:axId val="248141312"/>
+        <c:axId val="236563072"/>
+        <c:axId val="236564864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="248142848"/>
+        <c:axId val="236563072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1684,12 +1787,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="248141312"/>
+        <c:crossAx val="236564864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="248141312"/>
+        <c:axId val="236564864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1700,7 +1803,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="248142848"/>
+        <c:crossAx val="236563072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2010,11 +2113,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="248501376"/>
-        <c:axId val="248460032"/>
+        <c:axId val="236604032"/>
+        <c:axId val="236605824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="248501376"/>
+        <c:axId val="236604032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2024,12 +2127,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="248460032"/>
+        <c:crossAx val="236605824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="248460032"/>
+        <c:axId val="236605824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2040,7 +2143,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="248501376"/>
+        <c:crossAx val="236604032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2419,11 +2522,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="248900608"/>
-        <c:axId val="248899072"/>
+        <c:axId val="236641280"/>
+        <c:axId val="236659456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="248900608"/>
+        <c:axId val="236641280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2433,12 +2536,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="248899072"/>
+        <c:crossAx val="236659456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="248899072"/>
+        <c:axId val="236659456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2449,7 +2552,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="248900608"/>
+        <c:crossAx val="236641280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2999,11 +3102,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="246613120"/>
-        <c:axId val="245197440"/>
+        <c:axId val="236678528"/>
+        <c:axId val="236680320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="246613120"/>
+        <c:axId val="236678528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3013,12 +3116,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="245197440"/>
+        <c:crossAx val="236680320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="245197440"/>
+        <c:axId val="236680320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3029,7 +3132,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="246613120"/>
+        <c:crossAx val="236678528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3254,11 +3357,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="248201984"/>
-        <c:axId val="248200192"/>
+        <c:axId val="236278144"/>
+        <c:axId val="236279680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="248201984"/>
+        <c:axId val="236278144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3268,12 +3371,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="248200192"/>
+        <c:crossAx val="236279680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="248200192"/>
+        <c:axId val="236279680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3284,7 +3387,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="248201984"/>
+        <c:crossAx val="236278144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3320,6 +3423,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>genou d'appui, axe x</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -3654,37 +3776,85 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="236721664"/>
-        <c:axId val="236720128"/>
+        <c:axId val="162224000"/>
+        <c:axId val="162225536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="236721664"/>
+        <c:axId val="162224000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>niveau d'eau (en mètres)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1000">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="236720128"/>
+        <c:crossAx val="162225536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="236720128"/>
+        <c:axId val="162225536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>angle (en radians)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1000">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="236721664"/>
+        <c:crossAx val="162224000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3700,8 +3870,8 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="1.3149999999999999" header="0.3" footer="0.3"/>
+    <c:pageSetup paperSize="9" orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -4334,11 +4504,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="241413120"/>
-        <c:axId val="241411584"/>
+        <c:axId val="162266112"/>
+        <c:axId val="132523136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="241413120"/>
+        <c:axId val="162266112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4367,12 +4537,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="241411584"/>
+        <c:crossAx val="132523136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="241411584"/>
+        <c:axId val="132523136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4402,7 +4572,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="241413120"/>
+        <c:crossAx val="162266112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5156,11 +5326,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="166234752"/>
-        <c:axId val="166233216"/>
+        <c:axId val="168236160"/>
+        <c:axId val="168237696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="166234752"/>
+        <c:axId val="168236160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5170,12 +5340,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166233216"/>
+        <c:crossAx val="168237696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="166233216"/>
+        <c:axId val="168237696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5186,7 +5356,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166234752"/>
+        <c:crossAx val="168236160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5222,6 +5392,30 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>cheville d'appui,</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> axe x</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -5940,37 +6134,85 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="242728960"/>
-        <c:axId val="242714880"/>
+        <c:axId val="203055488"/>
+        <c:axId val="203057024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="242728960"/>
+        <c:axId val="203055488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>niveau d'eau (en mètres)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1000">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="242714880"/>
+        <c:crossAx val="203057024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="242714880"/>
+        <c:axId val="203057024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>angle (en radians)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1000">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="242728960"/>
+        <c:crossAx val="203055488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5986,8 +6228,8 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="1.3149999999999999" header="0.3" footer="0.3"/>
+    <c:pageSetup paperSize="9" orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -6006,6 +6248,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>pied en phase de vol, axe x</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -6212,37 +6473,85 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="248549376"/>
-        <c:axId val="247490816"/>
+        <c:axId val="203074560"/>
+        <c:axId val="203076352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="248549376"/>
+        <c:axId val="203074560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>niveau d'eau (en mètres)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1000">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="247490816"/>
+        <c:crossAx val="203076352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="247490816"/>
+        <c:axId val="203076352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>angle (en radians)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1000">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="248549376"/>
+        <c:crossAx val="203074560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6258,8 +6567,8 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="1.3149999999999999" header="0.3" footer="0.3"/>
+    <c:pageSetup paperSize="9" orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -6278,6 +6587,30 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>pied en phase de vol, axe y</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -6612,37 +6945,85 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="248423936"/>
-        <c:axId val="248422400"/>
+        <c:axId val="236006784"/>
+        <c:axId val="236012672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="248423936"/>
+        <c:axId val="236006784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>niveau d'eau (en mètres)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1000">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="248422400"/>
+        <c:crossAx val="236012672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="248422400"/>
+        <c:axId val="236012672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>angle (en radians)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1000">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="248423936"/>
+        <c:crossAx val="236006784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6658,8 +7039,8 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="1.3149999999999999" header="0.3" footer="0.3"/>
+    <c:pageSetup paperSize="9" orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -6693,7 +7074,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>φ=0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6757,7 +7138,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>φ=1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6769,8 +7150,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.36073731408573928"/>
-                  <c:y val="1.8043890347039952E-2"/>
+                  <c:x val="0.18557699037620298"/>
+                  <c:y val="0.14767351997666958"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -6834,43 +7215,90 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="237082496"/>
-        <c:axId val="237080960"/>
+        <c:axId val="236049152"/>
+        <c:axId val="236050688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="237082496"/>
+        <c:axId val="236049152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>niveau d'eau (en mètres)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="237080960"/>
+        <c:crossAx val="236050688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="237080960"/>
+        <c:axId val="236050688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1050" b="1" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>angle (en radians)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1050">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="237082496"/>
+        <c:crossAx val="236049152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
       <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
@@ -6880,8 +7308,8 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageMargins b="0" l="0" r="0" t="0" header="0" footer="0"/>
+    <c:pageSetup paperSize="121" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -6900,6 +7328,30 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>pied en phase de vol, axe z</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -7618,37 +8070,85 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="238693760"/>
-        <c:axId val="238691840"/>
+        <c:axId val="236389888"/>
+        <c:axId val="236391424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="238693760"/>
+        <c:axId val="236389888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>niveau d'eau (en mètres)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1000">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="238691840"/>
+        <c:crossAx val="236391424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="238691840"/>
+        <c:axId val="236391424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>angle (en radians)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1000">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="238693760"/>
+        <c:crossAx val="236389888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7664,8 +8164,8 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="1.3149999999999999" header="0.3" footer="0.3"/>
+    <c:pageSetup paperSize="9" orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -7825,14 +8325,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>42</xdr:col>
-      <xdr:colOff>213360</xdr:colOff>
-      <xdr:row>84</xdr:row>
+      <xdr:colOff>182880</xdr:colOff>
+      <xdr:row>88</xdr:row>
       <xdr:rowOff>22860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>48</xdr:col>
-      <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>99</xdr:row>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>103</xdr:row>
       <xdr:rowOff>22860</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -8452,8 +8952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BV82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BN73" workbookViewId="0">
-      <selection activeCell="M72" sqref="M72"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="BR86" sqref="BR86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8720,7 +9220,7 @@
         <v>1.621113</v>
       </c>
       <c r="G17">
-        <f>(F17+E17+D17+C17)/4</f>
+        <f t="shared" ref="G17:G27" si="0">(F17+E17+D17+C17)/4</f>
         <v>1.5087422500000001</v>
       </c>
       <c r="H17">
@@ -8747,7 +9247,7 @@
         <v>1.2610250000000001</v>
       </c>
       <c r="G18">
-        <f>(F18+E18+D18+C18)/4</f>
+        <f t="shared" si="0"/>
         <v>1.15714575</v>
       </c>
       <c r="H18">
@@ -8774,7 +9274,7 @@
         <v>1.294672</v>
       </c>
       <c r="G19">
-        <f>(F19+E19+D19+C19)/4</f>
+        <f t="shared" si="0"/>
         <v>1.2111144999999999</v>
       </c>
       <c r="H19">
@@ -8801,7 +9301,7 @@
         <v>0.38989000000000001</v>
       </c>
       <c r="G20">
-        <f>(F20+E20+D20+C20)/4</f>
+        <f t="shared" si="0"/>
         <v>0.54467224999999997</v>
       </c>
       <c r="H20">
@@ -8828,7 +9328,7 @@
         <v>9.7866999999999996E-2</v>
       </c>
       <c r="G21">
-        <f>(F21+E21+D21+C21)/4</f>
+        <f t="shared" si="0"/>
         <v>7.87495E-2</v>
       </c>
       <c r="H21">
@@ -8855,7 +9355,7 @@
         <v>-0.55203599999999997</v>
       </c>
       <c r="G22">
-        <f>(F22+E22+D22+C22)/4</f>
+        <f t="shared" si="0"/>
         <v>-0.33750174999999999</v>
       </c>
       <c r="H22">
@@ -8882,7 +9382,7 @@
         <v>3.7796999999999997E-2</v>
       </c>
       <c r="G23">
-        <f>(F23+E23+D23+C23)/4</f>
+        <f t="shared" si="0"/>
         <v>-7.8443499999999999E-2</v>
       </c>
       <c r="H23">
@@ -8909,7 +9409,7 @@
         <v>-0.80324600000000002</v>
       </c>
       <c r="G24">
-        <f>(F24+E24+D24+C24)/4</f>
+        <f t="shared" si="0"/>
         <v>-0.81335550000000001</v>
       </c>
       <c r="H24">
@@ -8936,7 +9436,7 @@
         <v>-0.33799299999999999</v>
       </c>
       <c r="G25">
-        <f>(F25+E25+D25+C25)/4</f>
+        <f t="shared" si="0"/>
         <v>-0.41681299999999999</v>
       </c>
       <c r="H25">
@@ -8963,7 +9463,7 @@
         <v>-0.79097700000000004</v>
       </c>
       <c r="G26">
-        <f>(F26+E26+D26+C26)/4</f>
+        <f t="shared" si="0"/>
         <v>-0.68371749999999998</v>
       </c>
       <c r="H26">
@@ -8990,7 +9490,7 @@
         <v>-3.9150000000000001E-3</v>
       </c>
       <c r="G27">
-        <f>(F27+E27+D27+C27)/4</f>
+        <f t="shared" si="0"/>
         <v>-0.17052675</v>
       </c>
       <c r="H27">
@@ -9917,11 +10417,11 @@
       <c r="BS77" t="s">
         <v>9</v>
       </c>
-      <c r="BU77">
-        <v>0</v>
-      </c>
-      <c r="BV77">
-        <v>1</v>
+      <c r="BU77" t="s">
+        <v>10</v>
+      </c>
+      <c r="BV77" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="78" spans="1:74" x14ac:dyDescent="0.3">
@@ -10845,7 +11345,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
backup before switching branch
</commit_message>
<xml_diff>
--- a/analyse_fonction_niveau_d'eau_07m_s.xlsx
+++ b/analyse_fonction_niveau_d'eau_07m_s.xlsx
@@ -405,11 +405,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="132163072"/>
-        <c:axId val="132164608"/>
+        <c:axId val="154334336"/>
+        <c:axId val="154336256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="132163072"/>
+        <c:axId val="154334336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -443,12 +443,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132164608"/>
+        <c:crossAx val="154336256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="132164608"/>
+        <c:axId val="154336256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -483,7 +483,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132163072"/>
+        <c:crossAx val="154334336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1033,11 +1033,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="236435328"/>
-        <c:axId val="236436864"/>
+        <c:axId val="172066688"/>
+        <c:axId val="172068224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="236435328"/>
+        <c:axId val="172066688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1047,12 +1047,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="236436864"/>
+        <c:crossAx val="172068224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="236436864"/>
+        <c:axId val="172068224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1063,14 +1063,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="236435328"/>
+        <c:crossAx val="172066688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1373,11 +1372,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="236525824"/>
-        <c:axId val="236527616"/>
+        <c:axId val="172173568"/>
+        <c:axId val="172175360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="236525824"/>
+        <c:axId val="172173568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1387,12 +1386,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="236527616"/>
+        <c:crossAx val="172175360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="236527616"/>
+        <c:axId val="172175360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1403,14 +1402,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="236525824"/>
+        <c:crossAx val="172173568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1773,11 +1771,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="236563072"/>
-        <c:axId val="236564864"/>
+        <c:axId val="172214912"/>
+        <c:axId val="172216704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="236563072"/>
+        <c:axId val="172214912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1787,12 +1785,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="236564864"/>
+        <c:crossAx val="172216704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="236564864"/>
+        <c:axId val="172216704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1803,14 +1801,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="236563072"/>
+        <c:crossAx val="172214912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2113,11 +2110,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="236604032"/>
-        <c:axId val="236605824"/>
+        <c:axId val="172239488"/>
+        <c:axId val="172241280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="236604032"/>
+        <c:axId val="172239488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2127,12 +2124,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="236605824"/>
+        <c:crossAx val="172241280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="236605824"/>
+        <c:axId val="172241280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2143,7 +2140,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="236604032"/>
+        <c:crossAx val="172239488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2522,11 +2519,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="236641280"/>
-        <c:axId val="236659456"/>
+        <c:axId val="172293120"/>
+        <c:axId val="172364544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="236641280"/>
+        <c:axId val="172293120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2536,12 +2533,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="236659456"/>
+        <c:crossAx val="172364544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="236659456"/>
+        <c:axId val="172364544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2552,14 +2549,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="236641280"/>
+        <c:crossAx val="172293120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3102,11 +3098,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="236678528"/>
-        <c:axId val="236680320"/>
+        <c:axId val="172412288"/>
+        <c:axId val="172414080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="236678528"/>
+        <c:axId val="172412288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3116,12 +3112,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="236680320"/>
+        <c:crossAx val="172414080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="236680320"/>
+        <c:axId val="172414080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3132,14 +3128,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="236678528"/>
+        <c:crossAx val="172412288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3357,11 +3352,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="236278144"/>
-        <c:axId val="236279680"/>
+        <c:axId val="172454272"/>
+        <c:axId val="172455808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="236278144"/>
+        <c:axId val="172454272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3371,12 +3366,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="236279680"/>
+        <c:crossAx val="172455808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="236279680"/>
+        <c:axId val="172455808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3387,14 +3382,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="236278144"/>
+        <c:crossAx val="172454272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3776,11 +3770,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="162224000"/>
-        <c:axId val="162225536"/>
+        <c:axId val="170887808"/>
+        <c:axId val="170910464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="162224000"/>
+        <c:axId val="170887808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3814,12 +3808,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="162225536"/>
+        <c:crossAx val="170910464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="162225536"/>
+        <c:axId val="170910464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3854,7 +3848,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="162224000"/>
+        <c:crossAx val="170887808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4504,11 +4498,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="162266112"/>
-        <c:axId val="132523136"/>
+        <c:axId val="171209856"/>
+        <c:axId val="171211776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="162266112"/>
+        <c:axId val="171209856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4530,19 +4524,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132523136"/>
+        <c:crossAx val="171211776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="132523136"/>
+        <c:axId val="171211776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4565,21 +4558,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="162266112"/>
+        <c:crossAx val="171209856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5326,11 +5317,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="168236160"/>
-        <c:axId val="168237696"/>
+        <c:axId val="171146240"/>
+        <c:axId val="171160320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="168236160"/>
+        <c:axId val="171146240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5340,12 +5331,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="168237696"/>
+        <c:crossAx val="171160320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="168237696"/>
+        <c:axId val="171160320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5356,14 +5347,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="168236160"/>
+        <c:crossAx val="171146240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5413,7 +5403,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -6134,11 +6123,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="203055488"/>
-        <c:axId val="203057024"/>
+        <c:axId val="171547264"/>
+        <c:axId val="171553536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="203055488"/>
+        <c:axId val="171547264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6165,19 +6154,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="203057024"/>
+        <c:crossAx val="171553536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="203057024"/>
+        <c:axId val="171553536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6205,21 +6193,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="203055488"/>
+        <c:crossAx val="171547264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6264,7 +6250,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -6473,11 +6458,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="203074560"/>
-        <c:axId val="203076352"/>
+        <c:axId val="171579648"/>
+        <c:axId val="171594112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="203074560"/>
+        <c:axId val="171579648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6504,19 +6489,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="203076352"/>
+        <c:crossAx val="171594112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="203076352"/>
+        <c:axId val="171594112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6544,21 +6528,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="203074560"/>
+        <c:crossAx val="171579648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6608,7 +6590,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -6945,11 +6926,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="236006784"/>
-        <c:axId val="236012672"/>
+        <c:axId val="171638784"/>
+        <c:axId val="171640704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="236006784"/>
+        <c:axId val="171638784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6976,19 +6957,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="236012672"/>
+        <c:crossAx val="171640704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="236012672"/>
+        <c:axId val="171640704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7016,21 +6996,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="236006784"/>
+        <c:crossAx val="171638784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7215,11 +7193,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="236049152"/>
-        <c:axId val="236050688"/>
+        <c:axId val="171677952"/>
+        <c:axId val="171684224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="236049152"/>
+        <c:axId val="171677952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7241,19 +7219,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="236050688"/>
+        <c:crossAx val="171684224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="236050688"/>
+        <c:axId val="171684224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7281,14 +7258,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="236049152"/>
+        <c:crossAx val="171677952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7299,7 +7275,6 @@
         <c:idx val="2"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7349,7 +7324,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -8070,11 +8044,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="236389888"/>
-        <c:axId val="236391424"/>
+        <c:axId val="172032384"/>
+        <c:axId val="172034304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="236389888"/>
+        <c:axId val="172032384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8101,19 +8075,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="236391424"/>
+        <c:crossAx val="172034304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="236391424"/>
+        <c:axId val="172034304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8141,21 +8114,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="236389888"/>
+        <c:crossAx val="172032384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8656,11 +8627,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="analyse_fonction_niveau_d'eau_07m_s_2" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="analyse_fonction_niveau_d'eau_07m_s_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="analyse_fonction_niveau_d'eau_07m_s_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="analyse_fonction_niveau_d'eau_07m_s_2" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8953,7 +8924,7 @@
   <dimension ref="A1:BV82"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="BR86" sqref="BR86"/>
+      <selection activeCell="G82" sqref="G82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>